<commit_message>
Manual testing of Experiment-Methodology-04 and aggreegation of the Consolidation Theory
</commit_message>
<xml_diff>
--- a/dev/Scrap.xlsx
+++ b/dev/Scrap.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gray/Projects/claude-code-bug-phantom-reads-17407/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D520F4D-DB4E-4649-A0BD-E5CA0074771F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF5FF9-B2B7-D34A-83E1-07FE7866CB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="88860" yWindow="8620" windowWidth="28040" windowHeight="17180" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
+    <workbookView xWindow="79780" yWindow="6260" windowWidth="34380" windowHeight="21800" activeTab="1" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiment-Methodology-04" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Token %</t>
   </si>
@@ -102,6 +103,72 @@
   </si>
   <si>
     <t>quick-reference.md</t>
+  </si>
+  <si>
+    <t>Pre-load Files</t>
+  </si>
+  <si>
+    <t>Dynamic Files</t>
+  </si>
+  <si>
+    <t>Token Count</t>
+  </si>
+  <si>
+    <t>docs/specs/operations-manual-standard.md</t>
+  </si>
+  <si>
+    <t>docs/specs/operations-manual-exceptions.md</t>
+  </si>
+  <si>
+    <t>docs/specs/architecture-deep-dive.md</t>
+  </si>
+  <si>
+    <t>docs/specs/troubleshooting-compendium.md</t>
+  </si>
+  <si>
+    <t>Read(docs/wpds/pipeline-refactor.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/data-pipeline-overview.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/module-alpha.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/module-beta.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/module-gamma.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/integration-layer.md)</t>
+  </si>
+  <si>
+    <t>Read(docs/specs/compliance-requirements.md)</t>
+  </si>
+  <si>
+    <t>size (bytes)</t>
+  </si>
+  <si>
+    <t>byte-to-tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokens -&gt; </t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bytes -&gt; </t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>.claude/commands/setup-hard.md</t>
+  </si>
+  <si>
+    <t>.claude/commands/analyze-wpd.md</t>
   </si>
 </sst>
 </file>
@@ -112,7 +179,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,13 +187,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,12 +221,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,16 +563,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733460C6-B2B9-A845-A0C9-A5529EFEB4F9}">
-  <dimension ref="A3:K24"/>
+  <dimension ref="A3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -969,8 +1054,459 @@
         <v>15840</v>
       </c>
     </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>962</v>
+      </c>
+      <c r="J25">
+        <v>19232</v>
+      </c>
+      <c r="K25">
+        <f>J25/200000</f>
+        <v>9.6159999999999995E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>2497</v>
+      </c>
+      <c r="J26">
+        <v>21988</v>
+      </c>
+      <c r="K26">
+        <f>J26/200000</f>
+        <v>0.10994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>1952</v>
+      </c>
+      <c r="J27">
+        <v>23941</v>
+      </c>
+      <c r="K27">
+        <f>J27/200000</f>
+        <v>0.11970500000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>2005</v>
+      </c>
+      <c r="J28">
+        <v>18088</v>
+      </c>
+      <c r="K28">
+        <f>J28/200000</f>
+        <v>9.0440000000000006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <f>SUM(I25:I28)</f>
+        <v>7416</v>
+      </c>
+      <c r="J29">
+        <f>SUM(J25:J28)</f>
+        <v>83249</v>
+      </c>
+      <c r="K29">
+        <f>SUM(K25:K28)</f>
+        <v>0.41624500000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FADC2A5-F0C5-254F-9660-50846ED4BEC2}">
+  <dimension ref="B2:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>402</v>
+      </c>
+      <c r="D3">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <v>1490</v>
+      </c>
+      <c r="G3">
+        <f>F3/C3</f>
+        <v>3.7064676616915424</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>618</v>
+      </c>
+      <c r="D4">
+        <v>63</v>
+      </c>
+      <c r="E4">
+        <f>SUM(C3:C4)</f>
+        <v>1020</v>
+      </c>
+      <c r="F4">
+        <v>2559</v>
+      </c>
+      <c r="G4">
+        <f>F4/C4</f>
+        <v>4.1407766990291259</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>19323</v>
+      </c>
+      <c r="D7">
+        <v>963</v>
+      </c>
+      <c r="F7">
+        <v>108497</v>
+      </c>
+      <c r="G7">
+        <f>F7/C7</f>
+        <v>5.614914868291673</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>15636</v>
+      </c>
+      <c r="D8">
+        <v>1593</v>
+      </c>
+      <c r="E8">
+        <f>SUM(C7:C8)</f>
+        <v>34959</v>
+      </c>
+      <c r="F8">
+        <v>66444</v>
+      </c>
+      <c r="G8">
+        <f>F8/C8</f>
+        <v>4.2494244052187264</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>14676</v>
+      </c>
+      <c r="D9">
+        <v>1071</v>
+      </c>
+      <c r="E9">
+        <f>SUM(C7:C9)</f>
+        <v>49635</v>
+      </c>
+      <c r="F9">
+        <v>85873</v>
+      </c>
+      <c r="G9">
+        <f>F9/C9</f>
+        <v>5.8512537476151536</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>18477</v>
+      </c>
+      <c r="D10">
+        <v>2006</v>
+      </c>
+      <c r="E10">
+        <f>SUM(C7:C10)</f>
+        <v>68112</v>
+      </c>
+      <c r="F10">
+        <v>83359</v>
+      </c>
+      <c r="G10">
+        <f>F10/C10</f>
+        <v>4.5115007847594306</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>5034</v>
+      </c>
+      <c r="D13">
+        <v>393</v>
+      </c>
+      <c r="F13">
+        <v>21978</v>
+      </c>
+      <c r="G13">
+        <f>F13/C13</f>
+        <v>4.365911799761621</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>6041</v>
+      </c>
+      <c r="D14">
+        <v>426</v>
+      </c>
+      <c r="F14">
+        <v>32350</v>
+      </c>
+      <c r="G14">
+        <f>F14/C14</f>
+        <v>5.3550736633007778</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>6204</v>
+      </c>
+      <c r="D15">
+        <v>743</v>
+      </c>
+      <c r="F15">
+        <v>24863</v>
+      </c>
+      <c r="G15">
+        <f>F15/C15</f>
+        <v>4.0075757575757578</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>6198</v>
+      </c>
+      <c r="D16">
+        <v>742</v>
+      </c>
+      <c r="F16">
+        <v>26029</v>
+      </c>
+      <c r="G16">
+        <f>F16/C16</f>
+        <v>4.1995805098418844</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>7658</v>
+      </c>
+      <c r="D17">
+        <v>772</v>
+      </c>
+      <c r="F17">
+        <v>33133</v>
+      </c>
+      <c r="G17">
+        <f>F17/C17</f>
+        <v>4.3265865761295377</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>4886</v>
+      </c>
+      <c r="D18">
+        <v>531</v>
+      </c>
+      <c r="F18">
+        <v>20349</v>
+      </c>
+      <c r="G18">
+        <f>F18/C18</f>
+        <v>4.1647564469914036</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>3939</v>
+      </c>
+      <c r="D19">
+        <v>393</v>
+      </c>
+      <c r="E19">
+        <f>SUM(C13:C19)</f>
+        <v>39960</v>
+      </c>
+      <c r="F19">
+        <v>18690</v>
+      </c>
+      <c r="G19">
+        <f>F19/C19</f>
+        <v>4.744859101294745</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C7:C10,C13:C19)</f>
+        <v>108072</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D7:D10,D13:D19)</f>
+        <v>9633</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F7:F10,F13:F19)</f>
+        <v>521565</v>
+      </c>
+      <c r="G21">
+        <f>F21/C21</f>
+        <v>4.8260881634465909</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="6">
+        <v>25000</v>
+      </c>
+      <c r="H24" s="4">
+        <f>G24*G21</f>
+        <v>120652.20408616477</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="6">
+        <v>66000</v>
+      </c>
+      <c r="H26" s="4">
+        <f>G26/G21</f>
+        <v>13675.672255615313</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added module-epsilon and module-phi to the repro scenario
</commit_message>
<xml_diff>
--- a/dev/Scrap.xlsx
+++ b/dev/Scrap.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gray/Projects/claude-code-bug-phantom-reads-17407/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF5FF9-B2B7-D34A-83E1-07FE7866CB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F871BB12-A3DC-F340-9B46-952C3BC4EB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="79780" yWindow="6260" windowWidth="34380" windowHeight="21800" activeTab="1" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
+    <workbookView xWindow="128600" yWindow="14820" windowWidth="24540" windowHeight="16940" activeTab="2" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Experiment-Methodology-04" sheetId="2" r:id="rId2"/>
+    <sheet name="Experiment-Methodology-04-build" sheetId="2" r:id="rId2"/>
+    <sheet name="Experiment-Methodology-04" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Token %</t>
   </si>
@@ -169,6 +170,39 @@
   </si>
   <si>
     <t>.claude/commands/analyze-wpd.md</t>
+  </si>
+  <si>
+    <t>.claude/commands/analyze-wpd-doc.md</t>
+  </si>
+  <si>
+    <t>docs/wpds/pipeline-refactor.md</t>
+  </si>
+  <si>
+    <t>docs/specs/data-pipeline-overview.md</t>
+  </si>
+  <si>
+    <t>docs/specs/module-alpha.md</t>
+  </si>
+  <si>
+    <t>docs/specs/module-beta.md</t>
+  </si>
+  <si>
+    <t>docs/specs/module-epsilon.md</t>
+  </si>
+  <si>
+    <t>docs/specs/module-gamma.md</t>
+  </si>
+  <si>
+    <t>docs/specs/module-phi.md</t>
+  </si>
+  <si>
+    <t>docs/specs/integration-layer.md</t>
+  </si>
+  <si>
+    <t>docs/specs/compliance-requirements.md</t>
+  </si>
+  <si>
+    <t>Command Files</t>
   </si>
 </sst>
 </file>
@@ -195,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -229,6 +269,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FADC2A5-F0C5-254F-9660-50846ED4BEC2}">
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1509,4 +1550,448 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D45E679-92F7-E54C-A372-A923E10CA380}">
+  <dimension ref="B2:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>402</v>
+      </c>
+      <c r="D3">
+        <v>51</v>
+      </c>
+      <c r="F3">
+        <v>1490</v>
+      </c>
+      <c r="G3">
+        <f>F3/C3</f>
+        <v>3.7064676616915424</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>655</v>
+      </c>
+      <c r="D4">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <f>SUM(C3:C4)</f>
+        <v>1057</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2559</v>
+      </c>
+      <c r="G4">
+        <f>F4/C4</f>
+        <v>3.9068702290076334</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>545</v>
+      </c>
+      <c r="D5">
+        <v>49</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1833</v>
+      </c>
+      <c r="G5">
+        <f>F5/C5</f>
+        <v>3.3633027522935781</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>19323</v>
+      </c>
+      <c r="D8">
+        <v>962</v>
+      </c>
+      <c r="F8">
+        <v>108497</v>
+      </c>
+      <c r="G8">
+        <f>F8/C8</f>
+        <v>5.614914868291673</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>15636</v>
+      </c>
+      <c r="D9">
+        <v>1592</v>
+      </c>
+      <c r="E9">
+        <f>SUM(C8:C9)</f>
+        <v>34959</v>
+      </c>
+      <c r="F9">
+        <v>66444</v>
+      </c>
+      <c r="G9">
+        <f>F9/C9</f>
+        <v>4.2494244052187264</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>14676</v>
+      </c>
+      <c r="D10">
+        <v>1070</v>
+      </c>
+      <c r="E10">
+        <f>SUM(C8:C10)</f>
+        <v>49635</v>
+      </c>
+      <c r="F10">
+        <v>85873</v>
+      </c>
+      <c r="G10">
+        <f>F10/C10</f>
+        <v>5.8512537476151536</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>18477</v>
+      </c>
+      <c r="D11">
+        <v>2005</v>
+      </c>
+      <c r="E11">
+        <f>SUM(C8:C11)</f>
+        <v>68112</v>
+      </c>
+      <c r="F11">
+        <v>83359</v>
+      </c>
+      <c r="G11">
+        <f>F11/C11</f>
+        <v>4.5115007847594306</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>5652</v>
+      </c>
+      <c r="D14">
+        <v>451</v>
+      </c>
+      <c r="F14" s="7">
+        <v>24869</v>
+      </c>
+      <c r="G14">
+        <f>F14/C14</f>
+        <v>4.4000353857041752</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>6732</v>
+      </c>
+      <c r="D15">
+        <v>459</v>
+      </c>
+      <c r="F15" s="7">
+        <v>35582</v>
+      </c>
+      <c r="G15">
+        <f>F15/C15</f>
+        <v>5.285502079619727</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>6204</v>
+      </c>
+      <c r="D16">
+        <v>742</v>
+      </c>
+      <c r="F16">
+        <v>24863</v>
+      </c>
+      <c r="G16">
+        <f>F16/C16</f>
+        <v>4.0075757575757578</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>6198</v>
+      </c>
+      <c r="D17">
+        <v>741</v>
+      </c>
+      <c r="F17">
+        <v>26029</v>
+      </c>
+      <c r="G17">
+        <f>F17/C17</f>
+        <v>4.1995805098418844</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>7666</v>
+      </c>
+      <c r="D18">
+        <v>875</v>
+      </c>
+      <c r="F18" s="7">
+        <v>29725</v>
+      </c>
+      <c r="G18">
+        <f>F18/C18</f>
+        <v>3.8775110879206887</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>7658</v>
+      </c>
+      <c r="D19">
+        <v>771</v>
+      </c>
+      <c r="F19">
+        <v>33133</v>
+      </c>
+      <c r="G19">
+        <f>F19/C19</f>
+        <v>4.3265865761295377</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20">
+        <v>7639</v>
+      </c>
+      <c r="D20">
+        <v>900</v>
+      </c>
+      <c r="F20" s="7">
+        <v>32088</v>
+      </c>
+      <c r="G20">
+        <f>F20/C20</f>
+        <v>4.2005498101845795</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>5532</v>
+      </c>
+      <c r="D21">
+        <v>631</v>
+      </c>
+      <c r="F21" s="7">
+        <v>22805</v>
+      </c>
+      <c r="G21">
+        <f>F21/C21</f>
+        <v>4.1223788864786695</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>3939</v>
+      </c>
+      <c r="D22">
+        <v>392</v>
+      </c>
+      <c r="E22">
+        <f>SUM(C14:C22)</f>
+        <v>57220</v>
+      </c>
+      <c r="F22">
+        <v>18690</v>
+      </c>
+      <c r="G22">
+        <f>F22/C22</f>
+        <v>4.744859101294745</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <f>SUM(C3:C5,C8:C11,C14:C22)</f>
+        <v>126934</v>
+      </c>
+      <c r="D24">
+        <f>SUM(D3:D5,D8:D11,D14:D22)</f>
+        <v>11755</v>
+      </c>
+      <c r="F24">
+        <f>SUM(F3:F5,F8:F11,F14:F22)</f>
+        <v>597839</v>
+      </c>
+      <c r="G24">
+        <f>F24/C24</f>
+        <v>4.7098413348669386</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G27" s="6">
+        <v>25000</v>
+      </c>
+      <c r="H27" s="4">
+        <f>G27*G24</f>
+        <v>117746.03337167346</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="6">
+        <v>66000</v>
+      </c>
+      <c r="H29" s="4">
+        <f>G29/G24</f>
+        <v>14013.210914644244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ran analysis on Experiments Barebones-216 and Barebones-2020. Discovered Anthropic may have fixed phantom reads issue. Additional investigations prepared.
</commit_message>
<xml_diff>
--- a/dev/Scrap.xlsx
+++ b/dev/Scrap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gray/Projects/claude-code-bug-phantom-reads-17407/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F871BB12-A3DC-F340-9B46-952C3BC4EB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E81725-41DC-0046-A2C8-D14673697447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="128600" yWindow="14820" windowWidth="24540" windowHeight="16940" activeTab="2" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
+    <workbookView xWindow="128680" yWindow="16800" windowWidth="24540" windowHeight="15100" activeTab="2" xr2:uid="{AA9C5E26-9D6E-1E43-B902-74000A46D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1557,7 +1557,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D22"/>
+      <selection activeCell="B8" sqref="B8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,6 +1637,10 @@
       <c r="D5">
         <v>49</v>
       </c>
+      <c r="E5">
+        <f>C3+C5</f>
+        <v>947</v>
+      </c>
       <c r="F5" s="7">
         <v>1833</v>
       </c>

</xml_diff>